<commit_message>
luatgm fix testcase and update usecase ID
</commit_message>
<xml_diff>
--- a/Test-Design-ver 1.0.xlsx
+++ b/Test-Design-ver 1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20358"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giap Minh Luat\Desktop\HCM\DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\do-an\QuyetTamPassDoAn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B6C83-BFB2-474B-BFB9-B126497D69B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99FD76A-D753-4F3A-9F05-3F1D6C974F1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1170,12 +1170,6 @@
     <t>Sprint1</t>
   </si>
   <si>
-    <t>Dashbroad</t>
-  </si>
-  <si>
-    <t>Total Human Resouce</t>
-  </si>
-  <si>
     <t>Employee managent</t>
   </si>
   <si>
@@ -1222,6 +1216,12 @@
   </si>
   <si>
     <t>Degree-DaskCertificate</t>
+  </si>
+  <si>
+    <t>Login,Logout</t>
+  </si>
+  <si>
+    <t>Employee Quantity</t>
   </si>
 </sst>
 </file>
@@ -3109,6 +3109,93 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3145,9 +3232,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3169,88 +3253,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="29" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3259,20 +3274,119 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="29" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="34" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3289,23 +3403,8 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="34" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="36" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3316,104 +3415,50 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3421,6 +3466,30 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3433,74 +3502,47 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3526,50 +3568,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="83" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="92" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="85" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3586,9 +3613,6 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="83" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="36" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3606,30 +3630,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="84" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="92" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3997,23 +3997,23 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="167"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="137"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="169"/>
+      <c r="C2" s="139"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -4029,10 +4029,10 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="138" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="169"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
@@ -4050,10 +4050,10 @@
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="138" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="169"/>
+      <c r="C4" s="139"/>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
@@ -4071,10 +4071,10 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="168" t="s">
+      <c r="B5" s="138" t="s">
         <v>178</v>
       </c>
-      <c r="C5" s="169"/>
+      <c r="C5" s="139"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
@@ -4089,24 +4089,24 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="170" t="s">
+      <c r="A6" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="172"/>
+      <c r="B6" s="141"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="142"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="173"/>
-      <c r="B7" s="174"/>
-      <c r="C7" s="174"/>
-      <c r="D7" s="174"/>
-      <c r="E7" s="174"/>
-      <c r="F7" s="174"/>
-      <c r="G7" s="175"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="10" t="s">
@@ -4121,10 +4121,10 @@
       <c r="D8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="176" t="s">
+      <c r="E8" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="177"/>
+      <c r="F8" s="147"/>
       <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
@@ -4142,10 +4142,10 @@
       <c r="D9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="178" t="s">
+      <c r="E9" s="148" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="179"/>
+      <c r="F9" s="149"/>
       <c r="G9" s="15" t="s">
         <v>176</v>
       </c>
@@ -4155,8 +4155,8 @@
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="179"/>
+      <c r="E10" s="148"/>
+      <c r="F10" s="149"/>
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7">
@@ -4164,8 +4164,8 @@
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="179"/>
+      <c r="E11" s="148"/>
+      <c r="F11" s="149"/>
       <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7">
@@ -4173,136 +4173,118 @@
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="179"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="149"/>
       <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A13" s="162" t="s">
+      <c r="A13" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="163"/>
-      <c r="C13" s="163"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="164"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="134"/>
     </row>
     <row r="14" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A14" s="152" t="s">
+      <c r="A14" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="153"/>
-      <c r="C14" s="154" t="s">
+      <c r="B14" s="151"/>
+      <c r="C14" s="152" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="155"/>
-      <c r="E14" s="153"/>
-      <c r="F14" s="154" t="s">
+      <c r="D14" s="153"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="156"/>
+      <c r="G14" s="154"/>
     </row>
     <row r="15" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="158"/>
-      <c r="C15" s="144" t="s">
+      <c r="B15" s="156"/>
+      <c r="C15" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="159"/>
-      <c r="E15" s="160"/>
-      <c r="F15" s="144" t="s">
+      <c r="D15" s="158"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="161"/>
+      <c r="G15" s="160"/>
     </row>
     <row r="16" spans="1:7" ht="39" customHeight="1">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="168" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="140"/>
-      <c r="C16" s="141" t="s">
+      <c r="B16" s="169"/>
+      <c r="C16" s="170" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="145"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="157"/>
+      <c r="G16" s="173"/>
     </row>
     <row r="17" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A17" s="139" t="s">
+      <c r="A17" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="140"/>
-      <c r="C17" s="146" t="s">
+      <c r="B17" s="169"/>
+      <c r="C17" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="142"/>
-      <c r="E17" s="143"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="145"/>
+      <c r="D17" s="171"/>
+      <c r="E17" s="172"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="173"/>
     </row>
     <row r="18" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A18" s="147" t="s">
+      <c r="A18" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="148"/>
-      <c r="C18" s="146" t="s">
+      <c r="B18" s="176"/>
+      <c r="C18" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="145"/>
+      <c r="D18" s="171"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="173"/>
     </row>
     <row r="19" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A19" s="147" t="s">
+      <c r="A19" s="175" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="148"/>
-      <c r="C19" s="149" t="s">
+      <c r="B19" s="176"/>
+      <c r="C19" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="150"/>
-      <c r="E19" s="151"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="179"/>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A20" s="132" t="s">
+      <c r="A20" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="133"/>
-      <c r="C20" s="134" t="s">
+      <c r="B20" s="162"/>
+      <c r="C20" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="135"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="138"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="166"/>
+      <c r="G20" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A6:G7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:G20"/>
@@ -4317,6 +4299,24 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:G7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" location="Traceability!A1" display="Traceability" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4348,20 +4348,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="180" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="183"/>
+      <c r="B2" s="181"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -4402,10 +4402,10 @@
       <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="183"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="28"/>
@@ -4418,12 +4418,12 @@
       <c r="B6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="184" t="s">
+      <c r="C6" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="186"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="183"/>
+      <c r="F6" s="184"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="32">
@@ -4432,12 +4432,12 @@
       <c r="B7" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="180" t="s">
+      <c r="C7" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="180"/>
-      <c r="E7" s="180"/>
-      <c r="F7" s="180"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="185"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="32">
@@ -4446,12 +4446,12 @@
       <c r="B8" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="180" t="s">
+      <c r="C8" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
+      <c r="D8" s="185"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="185"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="32">
@@ -4460,12 +4460,12 @@
       <c r="B9" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="180" t="s">
+      <c r="C9" s="185" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="180"/>
-      <c r="E9" s="180"/>
-      <c r="F9" s="180"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="185"/>
+      <c r="F9" s="185"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="32">
@@ -4474,12 +4474,12 @@
       <c r="B10" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="180" t="s">
+      <c r="C10" s="185" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="180"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="32">
@@ -4488,12 +4488,12 @@
       <c r="B11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="180" t="s">
+      <c r="C11" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="180"/>
+      <c r="D11" s="185"/>
+      <c r="E11" s="185"/>
+      <c r="F11" s="185"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="32">
@@ -4502,12 +4502,12 @@
       <c r="B12" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="180" t="s">
+      <c r="C12" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="180"/>
-      <c r="E12" s="180"/>
-      <c r="F12" s="180"/>
+      <c r="D12" s="185"/>
+      <c r="E12" s="185"/>
+      <c r="F12" s="185"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="32">
@@ -4516,12 +4516,12 @@
       <c r="B13" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="180" t="s">
+      <c r="C13" s="185" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="180"/>
-      <c r="E13" s="180"/>
-      <c r="F13" s="180"/>
+      <c r="D13" s="185"/>
+      <c r="E13" s="185"/>
+      <c r="F13" s="185"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="34">
@@ -4530,20 +4530,15 @@
       <c r="B14" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="181" t="s">
+      <c r="C14" s="186" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="181"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="181"/>
+      <c r="D14" s="186"/>
+      <c r="E14" s="186"/>
+      <c r="F14" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C14:F14"/>
@@ -4551,6 +4546,11 @@
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -4573,16 +4573,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="187" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="36"/>
@@ -4595,18 +4595,18 @@
       <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="221" t="s">
+      <c r="A3" s="189" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="194" t="s">
+      <c r="B3" s="191" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="223"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="196" t="s">
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="194" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="197"/>
+      <c r="F3" s="195"/>
       <c r="G3" s="39" t="s">
         <v>64</v>
       </c>
@@ -4615,18 +4615,18 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="222"/>
+      <c r="A4" s="190"/>
       <c r="B4" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="232" t="s">
+      <c r="C4" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="232"/>
-      <c r="E4" s="233" t="s">
+      <c r="D4" s="196"/>
+      <c r="E4" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="233" t="s">
+      <c r="F4" s="197" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="41">
@@ -4635,238 +4635,238 @@
       <c r="H4" s="42"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="221" t="s">
+      <c r="A5" s="189" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="191" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="223"/>
-      <c r="D5" s="195"/>
+      <c r="C5" s="192"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="196" t="s">
+      <c r="F5" s="194" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="224"/>
-      <c r="H5" s="225"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
     </row>
     <row r="6" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A6" s="192"/>
+      <c r="A6" s="204"/>
       <c r="B6" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="226" t="s">
+      <c r="C6" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="226" t="s">
+      <c r="D6" s="211" t="s">
         <v>70</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="211" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="227"/>
-      <c r="H6" s="228"/>
+      <c r="G6" s="212"/>
+      <c r="H6" s="213"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A7" s="192"/>
+      <c r="A7" s="204"/>
       <c r="B7" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="229" t="s">
+      <c r="C7" s="214" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="229" t="s">
+      <c r="D7" s="214" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="229" t="s">
+      <c r="F7" s="214" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="219"/>
-      <c r="H7" s="220"/>
+      <c r="G7" s="207"/>
+      <c r="H7" s="208"/>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1">
-      <c r="A8" s="222"/>
+      <c r="A8" s="190"/>
       <c r="B8" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="214" t="s">
+      <c r="C8" s="201" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="214" t="s">
+      <c r="D8" s="201" t="s">
         <v>76</v>
       </c>
       <c r="E8" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="214" t="s">
+      <c r="F8" s="201" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="215"/>
-      <c r="H8" s="216"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="203"/>
     </row>
     <row r="9" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A9" s="192"/>
-      <c r="B9" s="217" t="s">
+      <c r="A9" s="204"/>
+      <c r="B9" s="205" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="218"/>
-      <c r="D9" s="219" t="s">
+      <c r="C9" s="206"/>
+      <c r="D9" s="207" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="219"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="220"/>
+      <c r="E9" s="207"/>
+      <c r="F9" s="207"/>
+      <c r="G9" s="207"/>
+      <c r="H9" s="208"/>
     </row>
     <row r="10" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A10" s="192"/>
-      <c r="B10" s="217" t="s">
+      <c r="A10" s="204"/>
+      <c r="B10" s="205" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="218"/>
-      <c r="D10" s="211" t="s">
+      <c r="C10" s="206"/>
+      <c r="D10" s="198" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="212"/>
-      <c r="F10" s="212"/>
-      <c r="G10" s="212"/>
-      <c r="H10" s="213"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="199"/>
+      <c r="H10" s="200"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="219" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="49">
         <v>1</v>
       </c>
-      <c r="C11" s="207" t="s">
+      <c r="C11" s="221" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="207"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="207"/>
-      <c r="G11" s="207"/>
-      <c r="H11" s="208"/>
+      <c r="D11" s="221"/>
+      <c r="E11" s="221"/>
+      <c r="F11" s="221"/>
+      <c r="G11" s="221"/>
+      <c r="H11" s="222"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="206"/>
+      <c r="A12" s="220"/>
       <c r="B12" s="49">
         <v>2</v>
       </c>
-      <c r="C12" s="207" t="s">
+      <c r="C12" s="221" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="207"/>
-      <c r="E12" s="207"/>
-      <c r="F12" s="207"/>
-      <c r="G12" s="207"/>
-      <c r="H12" s="208"/>
+      <c r="D12" s="221"/>
+      <c r="E12" s="221"/>
+      <c r="F12" s="221"/>
+      <c r="G12" s="221"/>
+      <c r="H12" s="222"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="219" t="s">
         <v>83</v>
       </c>
       <c r="B13" s="49">
         <v>1</v>
       </c>
-      <c r="C13" s="207" t="s">
+      <c r="C13" s="221" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="207"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="207"/>
-      <c r="G13" s="207"/>
-      <c r="H13" s="208"/>
+      <c r="D13" s="221"/>
+      <c r="E13" s="221"/>
+      <c r="F13" s="221"/>
+      <c r="G13" s="221"/>
+      <c r="H13" s="222"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="206"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="50">
         <v>2</v>
       </c>
-      <c r="C14" s="209" t="s">
+      <c r="C14" s="223" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="209"/>
-      <c r="E14" s="209"/>
-      <c r="F14" s="209"/>
-      <c r="G14" s="209"/>
-      <c r="H14" s="210"/>
+      <c r="D14" s="223"/>
+      <c r="E14" s="223"/>
+      <c r="F14" s="223"/>
+      <c r="G14" s="223"/>
+      <c r="H14" s="224"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="191" t="s">
+      <c r="A15" s="229" t="s">
         <v>86</v>
       </c>
       <c r="B15" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="194" t="s">
+      <c r="C15" s="191" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="195"/>
+      <c r="D15" s="193"/>
       <c r="E15" s="43" t="s">
         <v>88</v>
       </c>
       <c r="F15" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="G15" s="196" t="s">
+      <c r="G15" s="194" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="197"/>
+      <c r="H15" s="195"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="192"/>
+      <c r="A16" s="204"/>
       <c r="B16" s="51">
         <v>1</v>
       </c>
-      <c r="C16" s="198" t="s">
+      <c r="C16" s="231" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="199"/>
+      <c r="D16" s="232"/>
       <c r="E16" s="52" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="52">
         <v>100</v>
       </c>
-      <c r="G16" s="200"/>
-      <c r="H16" s="199"/>
+      <c r="G16" s="233"/>
+      <c r="H16" s="232"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="192"/>
+      <c r="A17" s="204"/>
       <c r="B17" s="51">
         <v>2</v>
       </c>
-      <c r="C17" s="201" t="s">
+      <c r="C17" s="217" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="202"/>
+      <c r="D17" s="218"/>
       <c r="E17" s="53" t="s">
         <v>91</v>
       </c>
       <c r="F17" s="53">
         <v>100</v>
       </c>
-      <c r="G17" s="203"/>
-      <c r="H17" s="204"/>
+      <c r="G17" s="215"/>
+      <c r="H17" s="216"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="192"/>
+      <c r="A18" s="204"/>
       <c r="B18" s="51">
         <v>3</v>
       </c>
-      <c r="C18" s="201" t="s">
+      <c r="C18" s="217" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="202" t="s">
+      <c r="D18" s="218" t="s">
         <v>40</v>
       </c>
       <c r="E18" s="53" t="s">
@@ -4875,18 +4875,18 @@
       <c r="F18" s="53">
         <v>300</v>
       </c>
-      <c r="G18" s="203"/>
-      <c r="H18" s="204"/>
+      <c r="G18" s="215"/>
+      <c r="H18" s="216"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="192"/>
+      <c r="A19" s="204"/>
       <c r="B19" s="51">
         <v>4</v>
       </c>
-      <c r="C19" s="201" t="s">
+      <c r="C19" s="217" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="202" t="s">
+      <c r="D19" s="218" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="53" t="s">
@@ -4895,18 +4895,18 @@
       <c r="F19" s="53">
         <v>10</v>
       </c>
-      <c r="G19" s="203"/>
-      <c r="H19" s="204"/>
+      <c r="G19" s="215"/>
+      <c r="H19" s="216"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="192"/>
+      <c r="A20" s="204"/>
       <c r="B20" s="51">
         <v>5</v>
       </c>
-      <c r="C20" s="201" t="s">
+      <c r="C20" s="217" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="202" t="s">
+      <c r="D20" s="218" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="53" t="s">
@@ -4915,18 +4915,18 @@
       <c r="F20" s="53">
         <v>60</v>
       </c>
-      <c r="G20" s="203"/>
-      <c r="H20" s="204"/>
+      <c r="G20" s="215"/>
+      <c r="H20" s="216"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="192"/>
+      <c r="A21" s="204"/>
       <c r="B21" s="51">
         <v>6</v>
       </c>
-      <c r="C21" s="201" t="s">
+      <c r="C21" s="217" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="202" t="s">
+      <c r="D21" s="218" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="53" t="s">
@@ -4935,18 +4935,18 @@
       <c r="F21" s="53">
         <v>30</v>
       </c>
-      <c r="G21" s="203"/>
-      <c r="H21" s="204"/>
+      <c r="G21" s="215"/>
+      <c r="H21" s="216"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="192"/>
+      <c r="A22" s="204"/>
       <c r="B22" s="51">
         <v>7</v>
       </c>
-      <c r="C22" s="201" t="s">
+      <c r="C22" s="217" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="202" t="s">
+      <c r="D22" s="218" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="53" t="s">
@@ -4955,50 +4955,21 @@
       <c r="F22" s="53">
         <v>10</v>
       </c>
-      <c r="G22" s="203"/>
-      <c r="H22" s="204"/>
+      <c r="G22" s="215"/>
+      <c r="H22" s="216"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="193"/>
+      <c r="A23" s="230"/>
       <c r="B23" s="54"/>
-      <c r="C23" s="187"/>
-      <c r="D23" s="188"/>
+      <c r="C23" s="225"/>
+      <c r="D23" s="226"/>
       <c r="E23" s="55"/>
       <c r="F23" s="56"/>
-      <c r="G23" s="189"/>
-      <c r="H23" s="190"/>
+      <c r="G23" s="227"/>
+      <c r="H23" s="228"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="A15:A23"/>
@@ -5015,6 +4986,35 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5036,16 +5036,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="57"/>
@@ -5058,14 +5058,14 @@
       <c r="H2" s="57"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="260"/>
+      <c r="A3" s="240"/>
       <c r="B3" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="242" t="s">
+      <c r="C3" s="241" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="247"/>
+      <c r="D3" s="242"/>
       <c r="E3" s="59" t="s">
         <v>102</v>
       </c>
@@ -5080,14 +5080,14 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="260"/>
+      <c r="A4" s="240"/>
       <c r="B4" s="61">
         <v>1</v>
       </c>
-      <c r="C4" s="261" t="s">
+      <c r="C4" s="243" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="262"/>
+      <c r="D4" s="244"/>
       <c r="E4" s="62">
         <v>43739</v>
       </c>
@@ -5100,14 +5100,14 @@
       <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="260"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="65">
         <v>2</v>
       </c>
-      <c r="C5" s="256" t="s">
+      <c r="C5" s="236" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="257"/>
+      <c r="D5" s="237"/>
       <c r="E5" s="66">
         <v>43748</v>
       </c>
@@ -5120,14 +5120,14 @@
       <c r="H5" s="68"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="260"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="65">
         <v>3</v>
       </c>
-      <c r="C6" s="256" t="s">
+      <c r="C6" s="236" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="257"/>
+      <c r="D6" s="237"/>
       <c r="E6" s="66">
         <v>43748</v>
       </c>
@@ -5140,14 +5140,14 @@
       <c r="H6" s="68"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="260"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="65">
         <v>4</v>
       </c>
-      <c r="C7" s="256" t="s">
+      <c r="C7" s="236" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="257"/>
+      <c r="D7" s="237"/>
       <c r="E7" s="66">
         <v>43749</v>
       </c>
@@ -5160,14 +5160,14 @@
       <c r="H7" s="68"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="260"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="65">
         <v>5</v>
       </c>
-      <c r="C8" s="256" t="s">
+      <c r="C8" s="236" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="257"/>
+      <c r="D8" s="237"/>
       <c r="E8" s="66">
         <v>43749</v>
       </c>
@@ -5180,14 +5180,14 @@
       <c r="H8" s="68"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="260"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="65">
         <v>6</v>
       </c>
-      <c r="C9" s="256" t="s">
+      <c r="C9" s="236" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="257"/>
+      <c r="D9" s="237"/>
       <c r="E9" s="66">
         <v>43750</v>
       </c>
@@ -5200,14 +5200,14 @@
       <c r="H9" s="67"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="260"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="65">
         <v>7</v>
       </c>
-      <c r="C10" s="256" t="s">
+      <c r="C10" s="236" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="257"/>
+      <c r="D10" s="237"/>
       <c r="E10" s="66">
         <v>43750</v>
       </c>
@@ -5220,7 +5220,7 @@
       <c r="H10" s="68"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="260"/>
+      <c r="A11" s="240"/>
       <c r="B11" s="65"/>
       <c r="C11" s="69" t="s">
         <v>111</v>
@@ -5238,12 +5238,12 @@
       <c r="H11" s="68"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="260"/>
+      <c r="A12" s="240"/>
       <c r="B12" s="65"/>
-      <c r="C12" s="254" t="s">
+      <c r="C12" s="234" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="255"/>
+      <c r="D12" s="235"/>
       <c r="E12" s="66">
         <v>43750</v>
       </c>
@@ -5256,14 +5256,14 @@
       <c r="H12" s="68"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="260"/>
+      <c r="A13" s="240"/>
       <c r="B13" s="65">
         <v>8</v>
       </c>
-      <c r="C13" s="256" t="s">
+      <c r="C13" s="236" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="257"/>
+      <c r="D13" s="237"/>
       <c r="E13" s="66">
         <v>43753</v>
       </c>
@@ -5282,10 +5282,10 @@
       <c r="B14" s="65">
         <v>9</v>
       </c>
-      <c r="C14" s="256" t="s">
+      <c r="C14" s="236" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="257"/>
+      <c r="D14" s="237"/>
       <c r="E14" s="66">
         <v>43770</v>
       </c>
@@ -5302,10 +5302,10 @@
       <c r="B15" s="65">
         <v>10</v>
       </c>
-      <c r="C15" s="256" t="s">
+      <c r="C15" s="236" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="257"/>
+      <c r="D15" s="237"/>
       <c r="E15" s="66">
         <v>43814</v>
       </c>
@@ -5322,10 +5322,10 @@
       <c r="B16" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="242" t="s">
+      <c r="C16" s="241" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="247"/>
+      <c r="D16" s="242"/>
       <c r="E16" s="59" t="s">
         <v>118</v>
       </c>
@@ -5344,10 +5344,10 @@
       <c r="B17" s="75">
         <v>1</v>
       </c>
-      <c r="C17" s="248" t="s">
+      <c r="C17" s="245" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="249"/>
+      <c r="D17" s="246"/>
       <c r="E17" s="66">
         <v>43814</v>
       </c>
@@ -5364,10 +5364,10 @@
       <c r="B18" s="76">
         <v>2</v>
       </c>
-      <c r="C18" s="250" t="s">
+      <c r="C18" s="247" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="251"/>
+      <c r="D18" s="248"/>
       <c r="E18" s="66">
         <v>43814</v>
       </c>
@@ -5380,16 +5380,16 @@
       <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="234" t="s">
+      <c r="A19" s="249" t="s">
         <v>123</v>
       </c>
       <c r="B19" s="76">
         <v>3</v>
       </c>
-      <c r="C19" s="250" t="s">
+      <c r="C19" s="247" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="251"/>
+      <c r="D19" s="248"/>
       <c r="E19" s="66">
         <v>43814</v>
       </c>
@@ -5402,14 +5402,14 @@
       <c r="H19" s="68"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="235"/>
+      <c r="A20" s="250"/>
       <c r="B20" s="76">
         <v>4</v>
       </c>
-      <c r="C20" s="250" t="s">
+      <c r="C20" s="247" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="251"/>
+      <c r="D20" s="248"/>
       <c r="E20" s="66">
         <v>43814</v>
       </c>
@@ -5422,14 +5422,14 @@
       <c r="H20" s="68"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="235"/>
+      <c r="A21" s="250"/>
       <c r="B21" s="76">
         <v>5</v>
       </c>
-      <c r="C21" s="250" t="s">
+      <c r="C21" s="247" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="251"/>
+      <c r="D21" s="248"/>
       <c r="E21" s="66">
         <v>43814</v>
       </c>
@@ -5442,14 +5442,14 @@
       <c r="H21" s="68"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="235"/>
+      <c r="A22" s="250"/>
       <c r="B22" s="73">
         <v>6</v>
       </c>
-      <c r="C22" s="252" t="s">
+      <c r="C22" s="251" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="253"/>
+      <c r="D22" s="252"/>
       <c r="E22" s="66">
         <v>43814</v>
       </c>
@@ -5462,16 +5462,16 @@
       <c r="H22" s="74"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="234" t="s">
+      <c r="A23" s="249" t="s">
         <v>127</v>
       </c>
       <c r="B23" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="242" t="s">
+      <c r="C23" s="241" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="243"/>
+      <c r="D23" s="255"/>
       <c r="E23" s="77" t="s">
         <v>129</v>
       </c>
@@ -5486,14 +5486,14 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="25.5">
-      <c r="A24" s="240"/>
+      <c r="A24" s="253"/>
       <c r="B24" s="79">
         <v>1</v>
       </c>
-      <c r="C24" s="244" t="s">
+      <c r="C24" s="256" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="244"/>
+      <c r="D24" s="256"/>
       <c r="E24" s="80" t="s">
         <v>133</v>
       </c>
@@ -5508,14 +5508,14 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="51.75" customHeight="1">
-      <c r="A25" s="240"/>
+      <c r="A25" s="253"/>
       <c r="B25" s="79">
         <v>2</v>
       </c>
-      <c r="C25" s="245" t="s">
+      <c r="C25" s="257" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="246"/>
+      <c r="D25" s="258"/>
       <c r="E25" s="80" t="s">
         <v>148</v>
       </c>
@@ -5530,14 +5530,14 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" customHeight="1">
-      <c r="A26" s="240"/>
+      <c r="A26" s="253"/>
       <c r="B26" s="79">
         <v>3</v>
       </c>
-      <c r="C26" s="244" t="s">
+      <c r="C26" s="256" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="244"/>
+      <c r="D26" s="256"/>
       <c r="E26" s="80" t="s">
         <v>136</v>
       </c>
@@ -5552,14 +5552,14 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" customHeight="1">
-      <c r="A27" s="241"/>
+      <c r="A27" s="254"/>
       <c r="B27" s="79">
         <v>4</v>
       </c>
-      <c r="C27" s="244" t="s">
+      <c r="C27" s="256" t="s">
         <v>138</v>
       </c>
-      <c r="D27" s="244"/>
+      <c r="D27" s="256"/>
       <c r="E27" s="80" t="s">
         <v>139</v>
       </c>
@@ -5574,85 +5574,106 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="234" t="s">
+      <c r="A28" s="249" t="s">
         <v>140</v>
       </c>
       <c r="B28" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="236" t="s">
+      <c r="C28" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="236"/>
-      <c r="E28" s="236"/>
-      <c r="F28" s="236"/>
-      <c r="G28" s="236"/>
+      <c r="D28" s="259"/>
+      <c r="E28" s="259"/>
+      <c r="F28" s="259"/>
+      <c r="G28" s="259"/>
       <c r="H28" s="78" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="235"/>
+      <c r="A29" s="250"/>
       <c r="B29" s="84">
         <v>1</v>
       </c>
-      <c r="C29" s="237" t="s">
+      <c r="C29" s="260" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="237"/>
-      <c r="E29" s="237"/>
-      <c r="F29" s="237"/>
-      <c r="G29" s="237"/>
+      <c r="D29" s="260"/>
+      <c r="E29" s="260"/>
+      <c r="F29" s="260"/>
+      <c r="G29" s="260"/>
       <c r="H29" s="85"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="235"/>
+      <c r="A30" s="250"/>
       <c r="B30" s="86">
         <v>2</v>
       </c>
-      <c r="C30" s="237" t="s">
+      <c r="C30" s="260" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="237"/>
-      <c r="E30" s="237"/>
-      <c r="F30" s="237"/>
-      <c r="G30" s="237"/>
+      <c r="D30" s="260"/>
+      <c r="E30" s="260"/>
+      <c r="F30" s="260"/>
+      <c r="G30" s="260"/>
       <c r="H30" s="87"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="234" t="s">
+      <c r="A31" s="249" t="s">
         <v>143</v>
       </c>
       <c r="B31" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="236" t="s">
+      <c r="C31" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="236"/>
-      <c r="E31" s="236"/>
-      <c r="F31" s="236"/>
-      <c r="G31" s="236"/>
+      <c r="D31" s="259"/>
+      <c r="E31" s="259"/>
+      <c r="F31" s="259"/>
+      <c r="G31" s="259"/>
       <c r="H31" s="78" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="238"/>
+      <c r="A32" s="261"/>
       <c r="B32" s="88">
         <v>2</v>
       </c>
-      <c r="C32" s="239" t="s">
+      <c r="C32" s="262" t="s">
         <v>144</v>
       </c>
-      <c r="D32" s="239"/>
-      <c r="E32" s="239"/>
-      <c r="F32" s="239"/>
-      <c r="G32" s="239"/>
+      <c r="D32" s="262"/>
+      <c r="E32" s="262"/>
+      <c r="F32" s="262"/>
+      <c r="G32" s="262"/>
       <c r="H32" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -5667,27 +5688,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5708,15 +5708,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="267" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="279"/>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
+      <c r="B1" s="267"/>
+      <c r="C1" s="267"/>
+      <c r="D1" s="267"/>
+      <c r="E1" s="267"/>
+      <c r="F1" s="267"/>
+      <c r="G1" s="267"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="90"/>
@@ -5729,64 +5729,64 @@
     </row>
     <row r="3" spans="1:7" ht="19.5">
       <c r="A3" s="57"/>
-      <c r="B3" s="280" t="s">
+      <c r="B3" s="268" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="280"/>
-      <c r="D3" s="280"/>
-      <c r="E3" s="280"/>
-      <c r="F3" s="280"/>
-      <c r="G3" s="280"/>
+      <c r="C3" s="268"/>
+      <c r="D3" s="268"/>
+      <c r="E3" s="268"/>
+      <c r="F3" s="268"/>
+      <c r="G3" s="268"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="57"/>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281"/>
-      <c r="D4" s="281"/>
-      <c r="E4" s="281"/>
-      <c r="F4" s="281"/>
-      <c r="G4" s="281"/>
+      <c r="B4" s="269"/>
+      <c r="C4" s="269"/>
+      <c r="D4" s="269"/>
+      <c r="E4" s="269"/>
+      <c r="F4" s="269"/>
+      <c r="G4" s="269"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="57"/>
       <c r="B5" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="272" t="s">
+      <c r="C5" s="270" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="273"/>
-      <c r="E5" s="282" t="s">
+      <c r="D5" s="271"/>
+      <c r="E5" s="272" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="223"/>
-      <c r="G5" s="195"/>
+      <c r="F5" s="192"/>
+      <c r="G5" s="193"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="94"/>
       <c r="B6" s="95">
         <v>1</v>
       </c>
-      <c r="C6" s="283" t="s">
+      <c r="C6" s="273" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="275"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="199"/>
+      <c r="D6" s="274"/>
+      <c r="E6" s="275"/>
+      <c r="F6" s="276"/>
+      <c r="G6" s="232"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="94"/>
       <c r="B7" s="96">
         <v>2</v>
       </c>
-      <c r="C7" s="276" t="s">
+      <c r="C7" s="263" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="271"/>
-      <c r="E7" s="277"/>
-      <c r="F7" s="278"/>
-      <c r="G7" s="202"/>
+      <c r="D7" s="264"/>
+      <c r="E7" s="265"/>
+      <c r="F7" s="266"/>
+      <c r="G7" s="218"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="94"/>
@@ -5819,32 +5819,32 @@
       <c r="B10" s="97">
         <v>5</v>
       </c>
-      <c r="C10" s="263" t="s">
+      <c r="C10" s="277" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="264"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="266"/>
-      <c r="G10" s="267"/>
+      <c r="D10" s="278"/>
+      <c r="E10" s="279"/>
+      <c r="F10" s="280"/>
+      <c r="G10" s="281"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" s="268" t="s">
+      <c r="B12" s="282" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="268"/>
-      <c r="D12" s="268"/>
-      <c r="E12" s="268"/>
-      <c r="F12" s="268"/>
-      <c r="G12" s="268"/>
+      <c r="C12" s="282"/>
+      <c r="D12" s="282"/>
+      <c r="E12" s="282"/>
+      <c r="F12" s="282"/>
+      <c r="G12" s="282"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="272" t="s">
+      <c r="C13" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="273"/>
+      <c r="D13" s="271"/>
       <c r="E13" s="93" t="s">
         <v>88</v>
       </c>
@@ -5859,10 +5859,10 @@
       <c r="B14" s="98">
         <v>1</v>
       </c>
-      <c r="C14" s="274" t="s">
+      <c r="C14" s="285" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="275" t="s">
+      <c r="D14" s="274" t="s">
         <v>70</v>
       </c>
       <c r="E14" s="105" t="s">
@@ -5877,10 +5877,10 @@
       <c r="B15" s="98">
         <v>2</v>
       </c>
-      <c r="C15" s="270" t="s">
+      <c r="C15" s="284" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="271" t="s">
+      <c r="D15" s="264" t="s">
         <v>73</v>
       </c>
       <c r="E15" s="107" t="s">
@@ -5895,10 +5895,10 @@
       <c r="B16" s="98">
         <v>3</v>
       </c>
-      <c r="C16" s="270" t="s">
+      <c r="C16" s="284" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="271" t="s">
+      <c r="D16" s="264" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="107" t="s">
@@ -5913,10 +5913,10 @@
       <c r="B17" s="109">
         <v>4</v>
       </c>
-      <c r="C17" s="269" t="s">
+      <c r="C17" s="283" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="264" t="s">
+      <c r="D17" s="278" t="s">
         <v>160</v>
       </c>
       <c r="E17" s="110" t="s">
@@ -5929,6 +5929,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="A1:G1"/>
@@ -5938,14 +5946,6 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E9" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -5961,7 +5961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -5970,13 +5972,13 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="112"/>
-      <c r="B1" s="288" t="s">
+      <c r="B1" s="297" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="288"/>
-      <c r="D1" s="288"/>
-      <c r="E1" s="288"/>
-      <c r="F1" s="288"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
       <c r="G1" s="112"/>
       <c r="H1" s="112"/>
       <c r="I1" s="112"/>
@@ -6005,7 +6007,7 @@
       </c>
       <c r="C3" s="115">
         <f>J22</f>
-        <v>310</v>
+        <v>342</v>
       </c>
       <c r="D3" s="112"/>
       <c r="E3" s="112"/>
@@ -6046,41 +6048,41 @@
       <c r="L5" s="112"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="289" t="s">
+      <c r="A6" s="298" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="291" t="s">
+      <c r="B6" s="287" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="291" t="s">
+      <c r="C6" s="287" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="291" t="s">
+      <c r="D6" s="287" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="293" t="s">
+      <c r="E6" s="301" t="s">
         <v>167</v>
       </c>
-      <c r="F6" s="295" t="s">
+      <c r="F6" s="303" t="s">
         <v>168</v>
       </c>
-      <c r="G6" s="296"/>
-      <c r="H6" s="296"/>
-      <c r="I6" s="296"/>
-      <c r="J6" s="297"/>
-      <c r="K6" s="291" t="s">
+      <c r="G6" s="304"/>
+      <c r="H6" s="304"/>
+      <c r="I6" s="304"/>
+      <c r="J6" s="305"/>
+      <c r="K6" s="287" t="s">
         <v>63</v>
       </c>
-      <c r="L6" s="286" t="s">
+      <c r="L6" s="295" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="25.5">
-      <c r="A7" s="290"/>
-      <c r="B7" s="292"/>
-      <c r="C7" s="292"/>
-      <c r="D7" s="292"/>
-      <c r="E7" s="294"/>
+      <c r="A7" s="299"/>
+      <c r="B7" s="300"/>
+      <c r="C7" s="300"/>
+      <c r="D7" s="300"/>
+      <c r="E7" s="302"/>
       <c r="F7" s="116" t="s">
         <v>169</v>
       </c>
@@ -6096,15 +6098,15 @@
       <c r="J7" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="K7" s="299"/>
-      <c r="L7" s="287"/>
+      <c r="K7" s="288"/>
+      <c r="L7" s="296"/>
     </row>
     <row r="8" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A8" s="300" t="s">
+      <c r="A8" s="289" t="s">
         <v>183</v>
       </c>
       <c r="B8" s="127" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="C8" s="121">
         <v>1</v>
@@ -6112,24 +6114,24 @@
       <c r="D8" s="126"/>
       <c r="E8" s="118"/>
       <c r="F8" s="118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="118">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="118"/>
       <c r="I8" s="118"/>
       <c r="J8" s="119">
         <f t="shared" ref="J8:J10" si="0">SUM(F8:I8)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K8" s="124"/>
       <c r="L8" s="125"/>
     </row>
     <row r="9" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A9" s="301"/>
+      <c r="A9" s="290"/>
       <c r="B9" s="127" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C9" s="121">
         <v>2</v>
@@ -6152,9 +6154,9 @@
       <c r="L9" s="125"/>
     </row>
     <row r="10" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A10" s="301"/>
+      <c r="A10" s="290"/>
       <c r="B10" s="127" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10" s="121">
         <v>3</v>
@@ -6162,24 +6164,24 @@
       <c r="D10" s="126"/>
       <c r="E10" s="118"/>
       <c r="F10" s="118">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G10" s="118">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="118"/>
       <c r="I10" s="118"/>
       <c r="J10" s="119">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K10" s="124"/>
       <c r="L10" s="125"/>
     </row>
     <row r="11" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A11" s="302"/>
+      <c r="A11" s="291"/>
       <c r="B11" s="127" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C11" s="121">
         <v>4</v>
@@ -6190,23 +6192,23 @@
         <v>6</v>
       </c>
       <c r="G11" s="118">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="118"/>
       <c r="I11" s="118"/>
       <c r="J11" s="119">
         <f>SUM(F11:I11)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K11" s="117"/>
       <c r="L11" s="120"/>
     </row>
     <row r="12" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A12" s="298" t="s">
-        <v>188</v>
+      <c r="A12" s="286" t="s">
+        <v>186</v>
       </c>
       <c r="B12" s="127" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" s="121">
         <v>5</v>
@@ -6229,15 +6231,15 @@
       <c r="L12" s="125"/>
     </row>
     <row r="13" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A13" s="298"/>
-      <c r="B13" s="303" t="s">
-        <v>190</v>
+      <c r="A13" s="286"/>
+      <c r="B13" s="292" t="s">
+        <v>188</v>
       </c>
       <c r="C13" s="121">
         <v>6</v>
       </c>
       <c r="D13" s="126" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E13" s="118"/>
       <c r="F13" s="118">
@@ -6256,13 +6258,13 @@
       <c r="L13" s="125"/>
     </row>
     <row r="14" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A14" s="298"/>
-      <c r="B14" s="304"/>
+      <c r="A14" s="286"/>
+      <c r="B14" s="293"/>
       <c r="C14" s="121">
         <v>7</v>
       </c>
       <c r="D14" s="126" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E14" s="118"/>
       <c r="F14" s="118">
@@ -6281,13 +6283,13 @@
       <c r="L14" s="125"/>
     </row>
     <row r="15" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A15" s="298"/>
-      <c r="B15" s="305"/>
+      <c r="A15" s="286"/>
+      <c r="B15" s="294"/>
       <c r="C15" s="121">
         <v>8</v>
       </c>
       <c r="D15" s="126" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E15" s="118"/>
       <c r="F15" s="118">
@@ -6306,11 +6308,11 @@
       <c r="L15" s="125"/>
     </row>
     <row r="16" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A16" s="298" t="s">
-        <v>194</v>
+      <c r="A16" s="286" t="s">
+        <v>192</v>
       </c>
       <c r="B16" s="127" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16" s="121">
         <v>9</v>
@@ -6333,12 +6335,12 @@
       <c r="L16" s="125"/>
     </row>
     <row r="17" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A17" s="298"/>
+      <c r="A17" s="286"/>
       <c r="B17" s="127" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C17" s="121">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="126"/>
       <c r="E17" s="118"/>
@@ -6358,14 +6360,14 @@
       <c r="L17" s="120"/>
     </row>
     <row r="18" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A18" s="298" t="s">
-        <v>196</v>
+      <c r="A18" s="286" t="s">
+        <v>194</v>
       </c>
       <c r="B18" s="127" t="s">
         <v>174</v>
       </c>
       <c r="C18" s="121">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="126"/>
       <c r="E18" s="118"/>
@@ -6385,12 +6387,12 @@
       <c r="L18" s="125"/>
     </row>
     <row r="19" spans="1:12" ht="34.5" customHeight="1">
-      <c r="A19" s="298"/>
+      <c r="A19" s="286"/>
       <c r="B19" s="127" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" s="121">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="126"/>
       <c r="E19" s="118"/>
@@ -6410,14 +6412,14 @@
       <c r="L19" s="125"/>
     </row>
     <row r="20" spans="1:12" ht="38.25" customHeight="1">
-      <c r="A20" s="298" t="s">
-        <v>198</v>
+      <c r="A20" s="286" t="s">
+        <v>196</v>
       </c>
       <c r="B20" s="127" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" s="121">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="126"/>
       <c r="E20" s="118"/>
@@ -6437,12 +6439,12 @@
       <c r="L20" s="125"/>
     </row>
     <row r="21" spans="1:12" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A21" s="298"/>
+      <c r="A21" s="286"/>
       <c r="B21" s="127" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C21" s="121">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="126"/>
       <c r="E21" s="118"/>
@@ -6490,21 +6492,14 @@
       </c>
       <c r="I22" s="128"/>
       <c r="J22" s="128">
-        <f>SUM(J11:J21)</f>
-        <v>310</v>
+        <f>SUM(J8:J21)</f>
+        <v>342</v>
       </c>
       <c r="K22" s="122"/>
       <c r="L22" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A6:A7"/>
@@ -6513,6 +6508,13 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8:E21" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>